<commit_message>
datafile reproducing Kilian et al RD score regression results
</commit_message>
<xml_diff>
--- a/meta_regression_table.xlsx
+++ b/meta_regression_table.xlsx
@@ -8,22 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahkoenker/Dropbox/R Directory/DM Maps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D85F49-31DE-FB49-813F-87548AB14163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A5AA33-96E4-FA4D-A486-08A23E3943FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5980" yWindow="2800" windowWidth="31520" windowHeight="16260" xr2:uid="{BE022F06-25A3-6243-B0F6-A3AC2F3B5E9D}"/>
+    <workbookView xWindow="5980" yWindow="2800" windowWidth="31520" windowHeight="16260" activeTab="1" xr2:uid="{BE022F06-25A3-6243-B0F6-A3AC2F3B5E9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$3:$A$26</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$3:$B$26</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$4:$B$26</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$3</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$4:$C$26</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$B$3:$B$26</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$C$3:$C$26</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="70">
   <si>
     <t>Variable</t>
   </si>
@@ -184,13 +176,82 @@
   </si>
   <si>
     <t xml:space="preserve"> Mozambique</t>
+  </si>
+  <si>
+    <t>Adjusted Hazard Ratio (aHR)</t>
+  </si>
+  <si>
+    <t>Attitude never–SBC at least once</t>
+  </si>
+  <si>
+    <t>0.52–0.83</t>
+  </si>
+  <si>
+    <t>Attitude at least once–SBC never or at least once</t>
+  </si>
+  <si>
+    <t>0.45–0.70</t>
+  </si>
+  <si>
+    <t>Attitude at least twice–SBC at least twice</t>
+  </si>
+  <si>
+    <t>RD value/10 (impact of increase by 10 points of RD)</t>
+  </si>
+  <si>
+    <t>0.55–0.74</t>
+  </si>
+  <si>
+    <t>0.69–0.91</t>
+  </si>
+  <si>
+    <t>0.70–1.05</t>
+  </si>
+  <si>
+    <t>0.57–0.83</t>
+  </si>
+  <si>
+    <t>0.80–1.10</t>
+  </si>
+  <si>
+    <t>0.71–0.99</t>
+  </si>
+  <si>
+    <t>0.67–1.04</t>
+  </si>
+  <si>
+    <t>0.21–0.43</t>
+  </si>
+  <si>
+    <t>1.01–1.65</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Zanzibar (Tz)</t>
+  </si>
+  <si>
+    <t>0.34–0.73</t>
+  </si>
+  <si>
+    <t>Attitude</t>
+  </si>
+  <si>
+    <t>RD</t>
+  </si>
+  <si>
+    <t>Folding</t>
+  </si>
+  <si>
+    <t>Cooking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Mozambique</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -216,6 +277,25 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -256,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -292,6 +372,33 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -610,7 +717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{584C2028-3A61-E140-A3A2-8D1B4BB305F5}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -991,4 +1098,342 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7804C1A0-B3CA-684A-A0A2-B59E5A86D86E}">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="30.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="21">
+        <v>1</v>
+      </c>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="14">
+        <v>0.66</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="16">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="14">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="16">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="14">
+        <v>0.35</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="16">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="14">
+        <v>0.64</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="16">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="14">
+        <v>1.41</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="16">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="14">
+        <v>0.79</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="14">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="19">
+        <v>1</v>
+      </c>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="14">
+        <v>0.86</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="14">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="14">
+        <v>0.69</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="16">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="19">
+        <v>1</v>
+      </c>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+    </row>
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="14">
+        <v>0.94</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="14">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="14">
+        <v>0.84</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="14">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="19">
+        <v>1</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+    </row>
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="14">
+        <v>0.84</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="14">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="14">
+        <v>1</v>
+      </c>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+    </row>
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="16">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="14">
+        <v>1.29</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="14">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="16">
+        <v>1E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>